<commit_message>
Before model update -added table usersPerCompany
</commit_message>
<xml_diff>
--- a/Documents/ToDo/ToDo.xlsx
+++ b/Documents/ToDo/ToDo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Project C# en Java 2013-2014\C#\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\users\Ik\Documents\PHL\P3\Geintegreerd project\GIT\TogetherIsBetter\Documents\ToDo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ToDO!$A$1:$A$30</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -185,7 +185,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,8 +261,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,6 +321,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -377,7 +390,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -434,16 +447,20 @@
     <xf numFmtId="21" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="7" fillId="9" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="21" fontId="9" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="9" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="7" fillId="10" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Good" xfId="2" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Goed" xfId="2" builtinId="26"/>
+    <cellStyle name="Procent" xfId="1" builtinId="5"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="46">
     <dxf>
@@ -1031,7 +1048,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1164,7 +1181,7 @@
           <a:pPr rtl="0">
             <a:defRPr/>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1236,9 +1253,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1276,7 +1293,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1348,7 +1365,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1525,7 +1542,7 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1575,35 +1592,35 @@
       <c r="A2" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="44" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="43"/>
-      <c r="I2" s="41"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="40"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1">
       <c r="A3" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="44" t="s">
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="43"/>
-      <c r="I3" s="41"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="40"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="29" t="s">
@@ -1710,7 +1727,7 @@
       </c>
       <c r="C8" s="33"/>
       <c r="D8" s="33"/>
-      <c r="E8" s="34"/>
+      <c r="E8" s="44"/>
       <c r="F8" s="35"/>
       <c r="G8" s="36" t="s">
         <v>45</v>
@@ -1738,7 +1755,7 @@
       </c>
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
-      <c r="E9" s="34"/>
+      <c r="E9" s="44"/>
       <c r="F9" s="35"/>
       <c r="G9" s="36" t="s">
         <v>45</v>
@@ -1766,7 +1783,7 @@
       </c>
       <c r="C10" s="33"/>
       <c r="D10" s="33"/>
-      <c r="E10" s="34"/>
+      <c r="E10" s="44"/>
       <c r="F10" s="35"/>
       <c r="G10" s="36" t="s">
         <v>45</v>
@@ -1793,7 +1810,7 @@
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
-      <c r="E11" s="34"/>
+      <c r="E11" s="44"/>
       <c r="F11" s="35"/>
       <c r="G11" s="36" t="s">
         <v>45</v>
@@ -1810,7 +1827,7 @@
       </c>
       <c r="C12" s="33"/>
       <c r="D12" s="33"/>
-      <c r="E12" s="34"/>
+      <c r="E12" s="44"/>
       <c r="F12" s="35"/>
       <c r="G12" s="36" t="s">
         <v>45</v>
@@ -1878,10 +1895,10 @@
       </c>
       <c r="C16" s="35"/>
       <c r="D16" s="35"/>
-      <c r="E16" s="34"/>
+      <c r="E16" s="44"/>
       <c r="F16" s="35"/>
       <c r="G16" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H16" s="35"/>
       <c r="I16" s="35"/>
@@ -1890,7 +1907,7 @@
       <c r="A17" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="46" t="s">
         <v>29</v>
       </c>
       <c r="C17" s="35"/>
@@ -1912,7 +1929,7 @@
       </c>
       <c r="C18" s="35"/>
       <c r="D18" s="35"/>
-      <c r="E18" s="40"/>
+      <c r="E18" s="45"/>
       <c r="F18" s="35"/>
       <c r="G18" s="36" t="s">
         <v>45</v>
@@ -1929,7 +1946,7 @@
       </c>
       <c r="C19" s="35"/>
       <c r="D19" s="35"/>
-      <c r="E19" s="40"/>
+      <c r="E19" s="45"/>
       <c r="F19" s="35"/>
       <c r="G19" s="36" t="s">
         <v>45</v>
@@ -1946,7 +1963,7 @@
       </c>
       <c r="C20" s="35"/>
       <c r="D20" s="35"/>
-      <c r="E20" s="40"/>
+      <c r="E20" s="45"/>
       <c r="F20" s="35"/>
       <c r="G20" s="36" t="s">
         <v>45</v>
@@ -1963,7 +1980,7 @@
       </c>
       <c r="C21" s="35"/>
       <c r="D21" s="35"/>
-      <c r="E21" s="34"/>
+      <c r="E21" s="44"/>
       <c r="F21" s="35"/>
       <c r="G21" s="36" t="s">
         <v>45</v>
@@ -1980,7 +1997,7 @@
       </c>
       <c r="C22" s="35"/>
       <c r="D22" s="35"/>
-      <c r="E22" s="40"/>
+      <c r="E22" s="45"/>
       <c r="F22" s="35"/>
       <c r="G22" s="36" t="s">
         <v>45</v>
@@ -1997,7 +2014,7 @@
       </c>
       <c r="C23" s="35"/>
       <c r="D23" s="35"/>
-      <c r="E23" s="34"/>
+      <c r="E23" s="44"/>
       <c r="F23" s="35"/>
       <c r="G23" s="36" t="s">
         <v>45</v>
@@ -2014,7 +2031,7 @@
       </c>
       <c r="C24" s="35"/>
       <c r="D24" s="35"/>
-      <c r="E24" s="34"/>
+      <c r="E24" s="44"/>
       <c r="F24" s="35"/>
       <c r="G24" s="36" t="s">
         <v>45</v>
@@ -2031,7 +2048,7 @@
       </c>
       <c r="C25" s="35"/>
       <c r="D25" s="35"/>
-      <c r="E25" s="40"/>
+      <c r="E25" s="45"/>
       <c r="F25" s="35"/>
       <c r="G25" s="36" t="s">
         <v>45</v>
@@ -2048,7 +2065,7 @@
       </c>
       <c r="C26" s="35"/>
       <c r="D26" s="35"/>
-      <c r="E26" s="34"/>
+      <c r="E26" s="44"/>
       <c r="F26" s="35"/>
       <c r="G26" s="36" t="s">
         <v>45</v>
@@ -2082,7 +2099,7 @@
       </c>
       <c r="C28" s="35"/>
       <c r="D28" s="35"/>
-      <c r="E28" s="34"/>
+      <c r="E28" s="44"/>
       <c r="F28" s="35"/>
       <c r="G28" s="36" t="s">
         <v>45</v>
@@ -2099,7 +2116,7 @@
       </c>
       <c r="C29" s="35"/>
       <c r="D29" s="35"/>
-      <c r="E29" s="34"/>
+      <c r="E29" s="44"/>
       <c r="F29" s="35"/>
       <c r="G29" s="36" t="s">
         <v>45</v>
@@ -2111,7 +2128,7 @@
       <c r="A30" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="46" t="s">
         <v>42</v>
       </c>
       <c r="C30" s="35"/>
@@ -2133,7 +2150,7 @@
       </c>
       <c r="C31" s="35"/>
       <c r="D31" s="35"/>
-      <c r="E31" s="34"/>
+      <c r="E31" s="44"/>
       <c r="F31" s="35"/>
       <c r="G31" s="36" t="s">
         <v>45</v>

</xml_diff>